<commit_message>
Updeitnax rolite kato premaxnax georgi i moje bi razmestix po razli4en na4in ot tozi po koito se bqxme nagovorili trqbva da se pogledne. 4asti4no populnen User specification plan.
</commit_message>
<xml_diff>
--- a/I1/DevilerablesAndRoles2_Reworked.xlsx
+++ b/I1/DevilerablesAndRoles2_Reworked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Документи" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
   <si>
     <t> Наименование</t>
   </si>
@@ -256,12 +256,6 @@
   </si>
   <si>
     <t>Калоян</t>
-  </si>
-  <si>
-    <t>Георги</t>
-  </si>
-  <si>
-    <t>SA Manager</t>
   </si>
   <si>
     <t>Unit Tester</t>
@@ -903,7 +897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -981,10 +975,10 @@
         <v>13</v>
       </c>
       <c r="K3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="25" t="s">
         <v>83</v>
-      </c>
-      <c r="L3" s="25" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1008,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1043,7 +1037,7 @@
         <v>13</v>
       </c>
       <c r="K5" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
@@ -1079,7 +1073,7 @@
         <v>75</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1117,7 +1111,7 @@
         <v>5</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1143,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1244,10 +1238,10 @@
         <v>13</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1273,7 +1267,7 @@
         <v>75</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1339,7 +1333,7 @@
         <v>13</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1377,7 +1371,7 @@
         <v>4</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1440,7 +1434,7 @@
         <v>1.2</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1470,7 +1464,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1556,7 +1550,7 @@
         <v>2</v>
       </c>
       <c r="L21" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1644,7 +1638,7 @@
         <v>5</v>
       </c>
       <c r="L24" s="25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
@@ -1907,10 +1901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H10"/>
+  <dimension ref="C2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,11 +1913,10 @@
     <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="15">
         <v>1</v>
       </c>
@@ -1937,13 +1930,10 @@
         <v>4</v>
       </c>
       <c r="G2" s="15">
-        <v>5</v>
-      </c>
-      <c r="H2" s="15">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
         <v>74</v>
       </c>
@@ -1957,18 +1947,15 @@
         <v>76</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>71</v>
@@ -1977,15 +1964,12 @@
         <v>62</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>64</v>
@@ -1996,19 +1980,16 @@
       <c r="F5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>64</v>
@@ -2017,13 +1998,10 @@
         <v>64</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>77</v>
       </c>
@@ -2036,34 +2014,33 @@
       <c r="F7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="E8" s="12" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>